<commit_message>
Update the indoor experiment descriptions
</commit_message>
<xml_diff>
--- a/experiments/List of Experiments.xlsx
+++ b/experiments/List of Experiments.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1080" windowWidth="25600" windowHeight="14980" tabRatio="500"/>
+    <workbookView xWindow="300" yWindow="40" windowWidth="31300" windowHeight="20520" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="54">
   <si>
     <t>Line of sight distance tests</t>
   </si>
@@ -176,16 +176,34 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>Pick location for the Rpi, pick a path through the house</t>
+  </si>
+  <si>
+    <t>Repeat M and N at least once more time, preferably two more times</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -272,10 +290,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -309,23 +329,26 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -657,7 +680,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
@@ -667,20 +690,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="12"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="14"/>
     </row>
     <row r="2" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="12"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="14"/>
     </row>
     <row r="5" spans="1:21" ht="12.75" customHeight="1">
       <c r="A5" s="6" t="s">
@@ -688,53 +711,53 @@
       </c>
     </row>
     <row r="6" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
     </row>
     <row r="7" spans="1:21" ht="12.75" customHeight="1">
       <c r="A7" s="5"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13" t="s">
+      <c r="E7" s="12"/>
+      <c r="F7" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13" t="s">
+      <c r="G7" s="12"/>
+      <c r="H7" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13" t="s">
+      <c r="I7" s="12"/>
+      <c r="J7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13" t="s">
+      <c r="K7" s="12"/>
+      <c r="L7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13" t="s">
+      <c r="M7" s="12"/>
+      <c r="N7" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13" t="s">
+      <c r="O7" s="12"/>
+      <c r="P7" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="Q7" s="13"/>
-      <c r="R7" s="13" t="s">
+      <c r="Q7" s="12"/>
+      <c r="R7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="S7" s="13"/>
-      <c r="T7" s="13" t="s">
+      <c r="S7" s="12"/>
+      <c r="T7" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="U7" s="13"/>
+      <c r="U7" s="12"/>
     </row>
     <row r="8" spans="1:21" ht="12.75" customHeight="1">
       <c r="A8" s="10" t="s">
@@ -880,42 +903,42 @@
       <c r="A12" s="5"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13" t="s">
+      <c r="E12" s="12"/>
+      <c r="F12" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13" t="s">
+      <c r="G12" s="12"/>
+      <c r="H12" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13" t="s">
+      <c r="I12" s="12"/>
+      <c r="J12" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13" t="s">
+      <c r="K12" s="12"/>
+      <c r="L12" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="M12" s="13"/>
-      <c r="N12" s="13" t="s">
+      <c r="M12" s="12"/>
+      <c r="N12" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="O12" s="13"/>
-      <c r="P12" s="13" t="s">
+      <c r="O12" s="12"/>
+      <c r="P12" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="Q12" s="13"/>
-      <c r="R12" s="13" t="s">
+      <c r="Q12" s="12"/>
+      <c r="R12" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="S12" s="13"/>
-      <c r="T12" s="13" t="s">
+      <c r="S12" s="12"/>
+      <c r="T12" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="U12" s="13"/>
+      <c r="U12" s="12"/>
     </row>
     <row r="13" spans="1:21" ht="12.75" customHeight="1">
       <c r="A13" s="10" t="s">
@@ -1059,42 +1082,42 @@
       <c r="A17" s="5"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13" t="s">
+      <c r="E17" s="12"/>
+      <c r="F17" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13" t="s">
+      <c r="G17" s="12"/>
+      <c r="H17" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13" t="s">
+      <c r="I17" s="12"/>
+      <c r="J17" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13" t="s">
+      <c r="K17" s="12"/>
+      <c r="L17" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="M17" s="13"/>
-      <c r="N17" s="13" t="s">
+      <c r="M17" s="12"/>
+      <c r="N17" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="O17" s="13"/>
-      <c r="P17" s="13" t="s">
+      <c r="O17" s="12"/>
+      <c r="P17" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="Q17" s="13"/>
-      <c r="R17" s="13" t="s">
+      <c r="Q17" s="12"/>
+      <c r="R17" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="S17" s="13"/>
-      <c r="T17" s="13" t="s">
+      <c r="S17" s="12"/>
+      <c r="T17" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="U17" s="13"/>
+      <c r="U17" s="12"/>
     </row>
     <row r="18" spans="1:21" ht="12.75" customHeight="1">
       <c r="A18" s="10" t="s">
@@ -1238,42 +1261,42 @@
       <c r="A22" s="5"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13" t="s">
+      <c r="E22" s="12"/>
+      <c r="F22" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13" t="s">
+      <c r="G22" s="12"/>
+      <c r="H22" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13" t="s">
+      <c r="I22" s="12"/>
+      <c r="J22" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13" t="s">
+      <c r="K22" s="12"/>
+      <c r="L22" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13" t="s">
+      <c r="M22" s="12"/>
+      <c r="N22" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="O22" s="13"/>
-      <c r="P22" s="13" t="s">
+      <c r="O22" s="12"/>
+      <c r="P22" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="Q22" s="13"/>
-      <c r="R22" s="13" t="s">
+      <c r="Q22" s="12"/>
+      <c r="R22" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="S22" s="13"/>
-      <c r="T22" s="13" t="s">
+      <c r="S22" s="12"/>
+      <c r="T22" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="U22" s="13"/>
+      <c r="U22" s="12"/>
     </row>
     <row r="23" spans="1:21" ht="12.75" customHeight="1">
       <c r="A23" s="10" t="s">
@@ -1395,53 +1418,53 @@
     </row>
     <row r="27" spans="1:21" ht="12.75" customHeight="1">
       <c r="A27" s="5"/>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="12"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="14"/>
     </row>
     <row r="28" spans="1:21" ht="12.75" customHeight="1">
       <c r="A28" s="5"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
-      <c r="D28" s="13" t="s">
+      <c r="D28" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13" t="s">
+      <c r="E28" s="12"/>
+      <c r="F28" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13" t="s">
+      <c r="G28" s="12"/>
+      <c r="H28" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I28" s="13"/>
-      <c r="J28" s="13" t="s">
+      <c r="I28" s="12"/>
+      <c r="J28" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="K28" s="13"/>
-      <c r="L28" s="13" t="s">
+      <c r="K28" s="12"/>
+      <c r="L28" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="M28" s="13"/>
-      <c r="N28" s="13" t="s">
+      <c r="M28" s="12"/>
+      <c r="N28" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="O28" s="13"/>
-      <c r="P28" s="13" t="s">
+      <c r="O28" s="12"/>
+      <c r="P28" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="Q28" s="13"/>
-      <c r="R28" s="13" t="s">
+      <c r="Q28" s="12"/>
+      <c r="R28" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="S28" s="13"/>
-      <c r="T28" s="13" t="s">
+      <c r="S28" s="12"/>
+      <c r="T28" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="U28" s="13"/>
+      <c r="U28" s="12"/>
     </row>
     <row r="29" spans="1:21" ht="12.75" customHeight="1">
       <c r="A29" s="10" t="s">
@@ -1587,42 +1610,42 @@
       <c r="A33" s="5"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
-      <c r="D33" s="13" t="s">
+      <c r="D33" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13" t="s">
+      <c r="E33" s="12"/>
+      <c r="F33" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G33" s="13"/>
-      <c r="H33" s="13" t="s">
+      <c r="G33" s="12"/>
+      <c r="H33" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I33" s="13"/>
-      <c r="J33" s="13" t="s">
+      <c r="I33" s="12"/>
+      <c r="J33" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="K33" s="13"/>
-      <c r="L33" s="13" t="s">
+      <c r="K33" s="12"/>
+      <c r="L33" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="M33" s="13"/>
-      <c r="N33" s="13" t="s">
+      <c r="M33" s="12"/>
+      <c r="N33" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="O33" s="13"/>
-      <c r="P33" s="13" t="s">
+      <c r="O33" s="12"/>
+      <c r="P33" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="Q33" s="13"/>
-      <c r="R33" s="13" t="s">
+      <c r="Q33" s="12"/>
+      <c r="R33" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="S33" s="13"/>
-      <c r="T33" s="13" t="s">
+      <c r="S33" s="12"/>
+      <c r="T33" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="U33" s="13"/>
+      <c r="U33" s="12"/>
     </row>
     <row r="34" spans="1:21" ht="12.75" customHeight="1">
       <c r="A34" s="10" t="s">
@@ -1764,53 +1787,53 @@
     </row>
     <row r="38" spans="1:21" ht="12.75" customHeight="1">
       <c r="A38" s="5"/>
-      <c r="B38" s="11" t="s">
+      <c r="B38" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
     </row>
     <row r="39" spans="1:21" ht="12.75" customHeight="1">
       <c r="A39" s="5"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
-      <c r="D39" s="13" t="s">
+      <c r="D39" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13" t="s">
+      <c r="E39" s="12"/>
+      <c r="F39" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G39" s="13"/>
-      <c r="H39" s="13" t="s">
+      <c r="G39" s="12"/>
+      <c r="H39" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I39" s="13"/>
-      <c r="J39" s="13" t="s">
+      <c r="I39" s="12"/>
+      <c r="J39" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="K39" s="13"/>
-      <c r="L39" s="13" t="s">
+      <c r="K39" s="12"/>
+      <c r="L39" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="M39" s="13"/>
-      <c r="N39" s="13" t="s">
+      <c r="M39" s="12"/>
+      <c r="N39" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="O39" s="13"/>
-      <c r="P39" s="13" t="s">
+      <c r="O39" s="12"/>
+      <c r="P39" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="Q39" s="13"/>
-      <c r="R39" s="13" t="s">
+      <c r="Q39" s="12"/>
+      <c r="R39" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="S39" s="13"/>
-      <c r="T39" s="13" t="s">
+      <c r="S39" s="12"/>
+      <c r="T39" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="U39" s="13"/>
+      <c r="U39" s="12"/>
     </row>
     <row r="40" spans="1:21" ht="12.75" customHeight="1">
       <c r="A40" s="10" t="s">
@@ -1956,42 +1979,42 @@
       <c r="A44" s="5"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
-      <c r="D44" s="13" t="s">
+      <c r="D44" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13" t="s">
+      <c r="E44" s="12"/>
+      <c r="F44" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G44" s="13"/>
-      <c r="H44" s="13" t="s">
+      <c r="G44" s="12"/>
+      <c r="H44" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I44" s="13"/>
-      <c r="J44" s="13" t="s">
+      <c r="I44" s="12"/>
+      <c r="J44" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="K44" s="13"/>
-      <c r="L44" s="13" t="s">
+      <c r="K44" s="12"/>
+      <c r="L44" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="M44" s="13"/>
-      <c r="N44" s="13" t="s">
+      <c r="M44" s="12"/>
+      <c r="N44" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="O44" s="13"/>
-      <c r="P44" s="13" t="s">
+      <c r="O44" s="12"/>
+      <c r="P44" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="Q44" s="13"/>
-      <c r="R44" s="13" t="s">
+      <c r="Q44" s="12"/>
+      <c r="R44" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="S44" s="13"/>
-      <c r="T44" s="13" t="s">
+      <c r="S44" s="12"/>
+      <c r="T44" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="U44" s="13"/>
+      <c r="U44" s="12"/>
     </row>
     <row r="45" spans="1:21" ht="12.75" customHeight="1">
       <c r="A45" s="10" t="s">
@@ -2135,42 +2158,42 @@
       <c r="A49" s="5"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
-      <c r="D49" s="13" t="s">
+      <c r="D49" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13" t="s">
+      <c r="E49" s="12"/>
+      <c r="F49" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="G49" s="13"/>
-      <c r="H49" s="13" t="s">
+      <c r="G49" s="12"/>
+      <c r="H49" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="I49" s="13"/>
-      <c r="J49" s="13" t="s">
+      <c r="I49" s="12"/>
+      <c r="J49" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="K49" s="13"/>
-      <c r="L49" s="13" t="s">
+      <c r="K49" s="12"/>
+      <c r="L49" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="M49" s="13"/>
-      <c r="N49" s="13" t="s">
+      <c r="M49" s="12"/>
+      <c r="N49" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="O49" s="13"/>
-      <c r="P49" s="13" t="s">
+      <c r="O49" s="12"/>
+      <c r="P49" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="Q49" s="13"/>
-      <c r="R49" s="13" t="s">
+      <c r="Q49" s="12"/>
+      <c r="R49" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="S49" s="13"/>
-      <c r="T49" s="13" t="s">
+      <c r="S49" s="12"/>
+      <c r="T49" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="U49" s="13"/>
+      <c r="U49" s="12"/>
     </row>
     <row r="50" spans="1:21" ht="12.75" customHeight="1">
       <c r="A50" s="10" t="s">
@@ -2312,24 +2335,24 @@
     <row r="54" spans="1:21" ht="12.75" customHeight="1">
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
-      <c r="D54" s="14"/>
-      <c r="E54" s="14"/>
-      <c r="F54" s="14"/>
-      <c r="G54" s="14"/>
-      <c r="H54" s="14"/>
-      <c r="I54" s="14"/>
-      <c r="J54" s="14"/>
-      <c r="K54" s="14"/>
-      <c r="L54" s="14"/>
-      <c r="M54" s="14"/>
-      <c r="N54" s="14"/>
-      <c r="O54" s="14"/>
-      <c r="P54" s="14"/>
-      <c r="Q54" s="14"/>
-      <c r="R54" s="14"/>
-      <c r="S54" s="14"/>
-      <c r="T54" s="14"/>
-      <c r="U54" s="14"/>
+      <c r="D54" s="11"/>
+      <c r="E54" s="11"/>
+      <c r="F54" s="11"/>
+      <c r="G54" s="11"/>
+      <c r="H54" s="11"/>
+      <c r="I54" s="11"/>
+      <c r="J54" s="11"/>
+      <c r="K54" s="11"/>
+      <c r="L54" s="11"/>
+      <c r="M54" s="11"/>
+      <c r="N54" s="11"/>
+      <c r="O54" s="11"/>
+      <c r="P54" s="11"/>
+      <c r="Q54" s="11"/>
+      <c r="R54" s="11"/>
+      <c r="S54" s="11"/>
+      <c r="T54" s="11"/>
+      <c r="U54" s="11"/>
     </row>
     <row r="55" spans="1:21" ht="12.75" customHeight="1">
       <c r="B55" s="2"/>
@@ -2422,24 +2445,24 @@
     <row r="59" spans="1:21" ht="12.75" customHeight="1">
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
-      <c r="D59" s="14"/>
-      <c r="E59" s="14"/>
-      <c r="F59" s="14"/>
-      <c r="G59" s="14"/>
-      <c r="H59" s="14"/>
-      <c r="I59" s="14"/>
-      <c r="J59" s="14"/>
-      <c r="K59" s="14"/>
-      <c r="L59" s="14"/>
-      <c r="M59" s="14"/>
-      <c r="N59" s="14"/>
-      <c r="O59" s="14"/>
-      <c r="P59" s="14"/>
-      <c r="Q59" s="14"/>
-      <c r="R59" s="14"/>
-      <c r="S59" s="14"/>
-      <c r="T59" s="14"/>
-      <c r="U59" s="14"/>
+      <c r="D59" s="11"/>
+      <c r="E59" s="11"/>
+      <c r="F59" s="11"/>
+      <c r="G59" s="11"/>
+      <c r="H59" s="11"/>
+      <c r="I59" s="11"/>
+      <c r="J59" s="11"/>
+      <c r="K59" s="11"/>
+      <c r="L59" s="11"/>
+      <c r="M59" s="11"/>
+      <c r="N59" s="11"/>
+      <c r="O59" s="11"/>
+      <c r="P59" s="11"/>
+      <c r="Q59" s="11"/>
+      <c r="R59" s="11"/>
+      <c r="S59" s="11"/>
+      <c r="T59" s="11"/>
+      <c r="U59" s="11"/>
     </row>
     <row r="60" spans="1:21" ht="12.75" customHeight="1">
       <c r="B60" s="2"/>
@@ -2532,24 +2555,24 @@
     <row r="64" spans="1:21" ht="12.75" customHeight="1">
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
-      <c r="D64" s="14"/>
-      <c r="E64" s="14"/>
-      <c r="F64" s="14"/>
-      <c r="G64" s="14"/>
-      <c r="H64" s="14"/>
-      <c r="I64" s="14"/>
-      <c r="J64" s="14"/>
-      <c r="K64" s="14"/>
-      <c r="L64" s="14"/>
-      <c r="M64" s="14"/>
-      <c r="N64" s="14"/>
-      <c r="O64" s="14"/>
-      <c r="P64" s="14"/>
-      <c r="Q64" s="14"/>
-      <c r="R64" s="14"/>
-      <c r="S64" s="14"/>
-      <c r="T64" s="14"/>
-      <c r="U64" s="14"/>
+      <c r="D64" s="11"/>
+      <c r="E64" s="11"/>
+      <c r="F64" s="11"/>
+      <c r="G64" s="11"/>
+      <c r="H64" s="11"/>
+      <c r="I64" s="11"/>
+      <c r="J64" s="11"/>
+      <c r="K64" s="11"/>
+      <c r="L64" s="11"/>
+      <c r="M64" s="11"/>
+      <c r="N64" s="11"/>
+      <c r="O64" s="11"/>
+      <c r="P64" s="11"/>
+      <c r="Q64" s="11"/>
+      <c r="R64" s="11"/>
+      <c r="S64" s="11"/>
+      <c r="T64" s="11"/>
+      <c r="U64" s="11"/>
     </row>
     <row r="65" spans="2:21" ht="12.75" customHeight="1">
       <c r="B65" s="2"/>
@@ -2619,98 +2642,15 @@
     </row>
   </sheetData>
   <mergeCells count="113">
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="F64:G64"/>
-    <mergeCell ref="H64:I64"/>
-    <mergeCell ref="J64:K64"/>
-    <mergeCell ref="L64:M64"/>
-    <mergeCell ref="N64:O64"/>
-    <mergeCell ref="P64:Q64"/>
-    <mergeCell ref="R64:S64"/>
-    <mergeCell ref="T64:U64"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="F59:G59"/>
-    <mergeCell ref="H59:I59"/>
-    <mergeCell ref="J59:K59"/>
-    <mergeCell ref="L59:M59"/>
-    <mergeCell ref="N59:O59"/>
-    <mergeCell ref="P59:Q59"/>
-    <mergeCell ref="R59:S59"/>
-    <mergeCell ref="T59:U59"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="F54:G54"/>
-    <mergeCell ref="H54:I54"/>
-    <mergeCell ref="J54:K54"/>
-    <mergeCell ref="L54:M54"/>
-    <mergeCell ref="N54:O54"/>
-    <mergeCell ref="P54:Q54"/>
-    <mergeCell ref="R54:S54"/>
-    <mergeCell ref="T54:U54"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="H49:I49"/>
-    <mergeCell ref="J49:K49"/>
-    <mergeCell ref="L49:M49"/>
-    <mergeCell ref="N49:O49"/>
-    <mergeCell ref="P49:Q49"/>
-    <mergeCell ref="R49:S49"/>
-    <mergeCell ref="T49:U49"/>
-    <mergeCell ref="T39:U39"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="J44:K44"/>
-    <mergeCell ref="L44:M44"/>
-    <mergeCell ref="N44:O44"/>
-    <mergeCell ref="P44:Q44"/>
-    <mergeCell ref="R44:S44"/>
-    <mergeCell ref="T44:U44"/>
-    <mergeCell ref="B38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="J39:K39"/>
-    <mergeCell ref="L39:M39"/>
-    <mergeCell ref="N39:O39"/>
-    <mergeCell ref="P39:Q39"/>
-    <mergeCell ref="R39:S39"/>
-    <mergeCell ref="T28:U28"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="N33:O33"/>
-    <mergeCell ref="P33:Q33"/>
-    <mergeCell ref="R33:S33"/>
-    <mergeCell ref="T33:U33"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="L28:M28"/>
-    <mergeCell ref="N28:O28"/>
-    <mergeCell ref="P28:Q28"/>
-    <mergeCell ref="R28:S28"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="R22:S22"/>
-    <mergeCell ref="T22:U22"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="P17:Q17"/>
-    <mergeCell ref="R17:S17"/>
-    <mergeCell ref="T17:U17"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="N7:O7"/>
     <mergeCell ref="P7:Q7"/>
     <mergeCell ref="R7:S7"/>
     <mergeCell ref="T7:U7"/>
@@ -2723,15 +2663,98 @@
     <mergeCell ref="P12:Q12"/>
     <mergeCell ref="R12:S12"/>
     <mergeCell ref="T12:U12"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="R17:S17"/>
+    <mergeCell ref="T17:U17"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="R22:S22"/>
+    <mergeCell ref="T22:U22"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="L28:M28"/>
+    <mergeCell ref="N28:O28"/>
+    <mergeCell ref="P28:Q28"/>
+    <mergeCell ref="R28:S28"/>
+    <mergeCell ref="T28:U28"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="N33:O33"/>
+    <mergeCell ref="P33:Q33"/>
+    <mergeCell ref="R33:S33"/>
+    <mergeCell ref="T33:U33"/>
+    <mergeCell ref="B38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="L39:M39"/>
+    <mergeCell ref="N39:O39"/>
+    <mergeCell ref="P39:Q39"/>
+    <mergeCell ref="R39:S39"/>
+    <mergeCell ref="T39:U39"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="J44:K44"/>
+    <mergeCell ref="L44:M44"/>
+    <mergeCell ref="N44:O44"/>
+    <mergeCell ref="P44:Q44"/>
+    <mergeCell ref="R44:S44"/>
+    <mergeCell ref="T44:U44"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="H49:I49"/>
+    <mergeCell ref="J49:K49"/>
+    <mergeCell ref="L49:M49"/>
+    <mergeCell ref="N49:O49"/>
+    <mergeCell ref="P49:Q49"/>
+    <mergeCell ref="R49:S49"/>
+    <mergeCell ref="T49:U49"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="H54:I54"/>
+    <mergeCell ref="J54:K54"/>
+    <mergeCell ref="L54:M54"/>
+    <mergeCell ref="N54:O54"/>
+    <mergeCell ref="P54:Q54"/>
+    <mergeCell ref="R54:S54"/>
+    <mergeCell ref="T54:U54"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="H59:I59"/>
+    <mergeCell ref="J59:K59"/>
+    <mergeCell ref="L59:M59"/>
+    <mergeCell ref="N59:O59"/>
+    <mergeCell ref="P59:Q59"/>
+    <mergeCell ref="R59:S59"/>
+    <mergeCell ref="T59:U59"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="H64:I64"/>
+    <mergeCell ref="J64:K64"/>
+    <mergeCell ref="L64:M64"/>
+    <mergeCell ref="N64:O64"/>
+    <mergeCell ref="P64:Q64"/>
+    <mergeCell ref="R64:S64"/>
+    <mergeCell ref="T64:U64"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -2744,9 +2767,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U28"/>
+  <dimension ref="A1:U30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
@@ -2754,61 +2779,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
     </row>
     <row r="3" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
     </row>
     <row r="4" spans="1:21" ht="12.75" customHeight="1">
       <c r="A4" s="5"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13" t="s">
+      <c r="E4" s="12"/>
+      <c r="F4" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13" t="s">
+      <c r="G4" s="12"/>
+      <c r="H4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13" t="s">
+      <c r="I4" s="12"/>
+      <c r="J4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13" t="s">
+      <c r="K4" s="12"/>
+      <c r="L4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13" t="s">
+      <c r="M4" s="12"/>
+      <c r="N4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13" t="s">
+      <c r="O4" s="12"/>
+      <c r="P4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="Q4" s="13"/>
-      <c r="R4" s="13" t="s">
+      <c r="Q4" s="12"/>
+      <c r="R4" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="S4" s="13"/>
-      <c r="T4" s="13" t="s">
+      <c r="S4" s="12"/>
+      <c r="T4" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="U4" s="13"/>
+      <c r="U4" s="12"/>
     </row>
     <row r="5" spans="1:21" ht="12.75" customHeight="1">
       <c r="A5" s="10" t="s">
@@ -2954,42 +2979,42 @@
       <c r="A9" s="5"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13" t="s">
+      <c r="E9" s="12"/>
+      <c r="F9" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13" t="s">
+      <c r="G9" s="12"/>
+      <c r="H9" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13" t="s">
+      <c r="I9" s="12"/>
+      <c r="J9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13" t="s">
+      <c r="K9" s="12"/>
+      <c r="L9" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13" t="s">
+      <c r="M9" s="12"/>
+      <c r="N9" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="O9" s="13"/>
-      <c r="P9" s="13" t="s">
+      <c r="O9" s="12"/>
+      <c r="P9" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="Q9" s="13"/>
-      <c r="R9" s="13" t="s">
+      <c r="Q9" s="12"/>
+      <c r="R9" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="S9" s="13"/>
-      <c r="T9" s="13" t="s">
+      <c r="S9" s="12"/>
+      <c r="T9" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="U9" s="13"/>
+      <c r="U9" s="12"/>
     </row>
     <row r="10" spans="1:21" ht="12.75" customHeight="1">
       <c r="A10" s="10" t="s">
@@ -3133,42 +3158,42 @@
       <c r="A14" s="5"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13" t="s">
+      <c r="E14" s="12"/>
+      <c r="F14" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13" t="s">
+      <c r="G14" s="12"/>
+      <c r="H14" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13" t="s">
+      <c r="I14" s="12"/>
+      <c r="J14" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13" t="s">
+      <c r="K14" s="12"/>
+      <c r="L14" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="M14" s="13"/>
-      <c r="N14" s="13" t="s">
+      <c r="M14" s="12"/>
+      <c r="N14" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="O14" s="13"/>
-      <c r="P14" s="13" t="s">
+      <c r="O14" s="12"/>
+      <c r="P14" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="Q14" s="13"/>
-      <c r="R14" s="13" t="s">
+      <c r="Q14" s="12"/>
+      <c r="R14" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="S14" s="13"/>
-      <c r="T14" s="13" t="s">
+      <c r="S14" s="12"/>
+      <c r="T14" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="U14" s="13"/>
+      <c r="U14" s="12"/>
     </row>
     <row r="15" spans="1:21" ht="12.75" customHeight="1">
       <c r="A15" s="10" t="s">
@@ -3325,49 +3350,49 @@
       <c r="A21" s="5"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13" t="s">
+      <c r="E21" s="12"/>
+      <c r="F21" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13" t="s">
+      <c r="G21" s="12"/>
+      <c r="H21" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13" t="s">
+      <c r="I21" s="12"/>
+      <c r="J21" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13" t="s">
+      <c r="K21" s="12"/>
+      <c r="L21" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13" t="s">
+      <c r="M21" s="12"/>
+      <c r="N21" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="O21" s="13"/>
-      <c r="P21" s="13" t="s">
+      <c r="O21" s="12"/>
+      <c r="P21" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="Q21" s="13"/>
-      <c r="R21" s="13" t="s">
+      <c r="Q21" s="12"/>
+      <c r="R21" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="S21" s="13"/>
-      <c r="T21" s="13" t="s">
+      <c r="S21" s="12"/>
+      <c r="T21" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="U21" s="13"/>
+      <c r="U21" s="12"/>
     </row>
     <row r="22" spans="1:21" ht="12.75" customHeight="1">
       <c r="A22" s="10" t="s">
         <v>50</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>15</v>
@@ -3483,49 +3508,49 @@
       <c r="A25" s="5"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
-      <c r="D25" s="13" t="s">
+      <c r="D25" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13" t="s">
+      <c r="E25" s="12"/>
+      <c r="F25" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13" t="s">
+      <c r="G25" s="12"/>
+      <c r="H25" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13" t="s">
+      <c r="I25" s="12"/>
+      <c r="J25" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13" t="s">
+      <c r="K25" s="12"/>
+      <c r="L25" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="M25" s="13"/>
-      <c r="N25" s="13" t="s">
+      <c r="M25" s="12"/>
+      <c r="N25" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="O25" s="13"/>
-      <c r="P25" s="13" t="s">
+      <c r="O25" s="12"/>
+      <c r="P25" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="Q25" s="13"/>
-      <c r="R25" s="13" t="s">
+      <c r="Q25" s="12"/>
+      <c r="R25" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="S25" s="13"/>
-      <c r="T25" s="13" t="s">
+      <c r="S25" s="12"/>
+      <c r="T25" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="U25" s="13"/>
+      <c r="U25" s="12"/>
     </row>
     <row r="26" spans="1:21" ht="12.75" customHeight="1">
       <c r="A26" s="10" t="s">
         <v>51</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>15</v>
@@ -3636,8 +3661,45 @@
       <c r="T28" s="1"/>
       <c r="U28" s="1"/>
     </row>
+    <row r="30" spans="1:21" ht="12.75" customHeight="1">
+      <c r="A30" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="T4:U4"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="R9:S9"/>
+    <mergeCell ref="T9:U9"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="T14:U14"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="R14:S14"/>
     <mergeCell ref="N21:O21"/>
     <mergeCell ref="P21:Q21"/>
     <mergeCell ref="R21:S21"/>
@@ -3654,40 +3716,9 @@
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="F21:G21"/>
     <mergeCell ref="H21:I21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="R14:S14"/>
-    <mergeCell ref="T14:U14"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="L14:M14"/>
-    <mergeCell ref="T4:U4"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="R9:S9"/>
-    <mergeCell ref="T9:U9"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>